<commit_message>
Pequenas mudanças e correções de erros
</commit_message>
<xml_diff>
--- a/LogicaDeProgramacao/Java/Trabalho/EP-190_ Desenvolvimento do Protótipo de um Sistema de Gerenciamento de Estoque (SGE) (2).xlsx
+++ b/LogicaDeProgramacao/Java/Trabalho/EP-190_ Desenvolvimento do Protótipo de um Sistema de Gerenciamento de Estoque (SGE) (2).xlsx
@@ -729,24 +729,19 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -754,6 +749,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -762,12 +758,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,8 +1062,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:K22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1083,9 +1083,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.4">
-      <c r="A1" s="29"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
@@ -1111,18 +1111,18 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.4">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
       <c r="E2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="15.6">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
@@ -1132,62 +1132,62 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="E4" s="3"/>
       <c r="G4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="14.4">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="E5" s="3"/>
       <c r="G5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="37"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="39" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="37"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1199,12 +1199,12 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1216,47 +1216,47 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="40" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:26" ht="5.25" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
     </row>
     <row r="12" spans="1:26" ht="14.4">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1333,49 +1333,49 @@
       <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="14.4">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="37"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
     </row>
     <row r="19" spans="1:11" ht="111" customHeight="1">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="46"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:11" ht="5.25" customHeight="1">
       <c r="A20" s="24"/>
@@ -1391,34 +1391,34 @@
       <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="37"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="234.75" customHeight="1">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="37"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
     </row>
     <row r="23" spans="1:11" ht="5.25" customHeight="1">
       <c r="A23" s="24"/>
@@ -1434,34 +1434,34 @@
       <c r="K23" s="25"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="37"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
     </row>
     <row r="25" spans="1:11" ht="162" customHeight="1">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="37"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="24"/>
@@ -9277,6 +9277,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:C5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A22:K22"/>
@@ -9289,15 +9294,10 @@
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A1:C5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>